<commit_message>
feedback: Fix milk-burundi excel
Column name was not right, so we were putting 0 everywhere
</commit_message>
<xml_diff>
--- a/data/milk-burundi/milk-burundi-eco.xlsx
+++ b/data/milk-burundi/milk-burundi-eco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Value Chain" sheetId="1" state="visible" r:id="rId3"/>
@@ -311,7 +311,7 @@
     <t xml:space="preserve">Actor type Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Number Of actors In the value chain</t>
+    <t xml:space="preserve">Number of actors in the value chain</t>
   </si>
   <si>
     <t xml:space="preserve">Direct added value (local currency)</t>
@@ -493,7 +493,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,6 +516,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -643,7 +647,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -5034,8 +5038,8 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5050,7 +5054,7 @@
       <c r="B1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D1" s="2" t="s">

</xml_diff>